<commit_message>
Added in runtime temporary folder locations which will delete before each application start as well as before each transaction
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lande\OneDrive\Documents\UiPath\PathFindr-RoboticEnterpriseFramework\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AD1ED3-B53E-4E60-B03B-8356F1F847F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E4A6A6-E3E6-498B-9C48-7B315B3A2165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39540" yWindow="2640" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -159,7 +159,25 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>Test Queue</t>
+  </si>
+  <si>
+    <t>Data/Temp/Temp Application</t>
+  </si>
+  <si>
+    <t>TempApplicationFolder</t>
+  </si>
+  <si>
+    <t>TempTransactionFolder</t>
+  </si>
+  <si>
+    <t>Data/Temp/Temp Transaction</t>
+  </si>
+  <si>
+    <t>A temporary folder path that will get cleaned up right before InitAllApplications. This is beneficial in storing temporary data that should last the lifetime of a single application run</t>
+  </si>
+  <si>
+    <t>A temporary folder path that will get cleaned up right before Process. This is beneficial in storing temporary data that should last the lifetime of a single transaction</t>
   </si>
 </sst>
 </file>
@@ -538,7 +556,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1619,8 +1637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1801,8 +1819,28 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="51" customHeight="1">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2782,7 +2820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>

</xml_diff>